<commit_message>
Resolve issues for Histogram
</commit_message>
<xml_diff>
--- a/documents/Published/HistogramXY/HistogramXYByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/HistogramXY/HistogramXYByMAQSoftwareChecklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunny\Desktop\HistogramXY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualWork\documents\Published\HistogramXY\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>S no</t>
   </si>
@@ -288,6 +288,19 @@
   </si>
   <si>
     <t>Does visual legends adjusted on resizing? </t>
+  </si>
+  <si>
+    <t>X axis</t>
+  </si>
+  <si>
+    <t>Added start and end fields.</t>
+  </si>
+  <si>
+    <t>1. Enter value for Start field
+2. Enter value for End field</t>
+  </si>
+  <si>
+    <t>Histogram Chart will be displayed with specified start and end values.</t>
   </si>
 </sst>
 </file>
@@ -419,31 +432,31 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -769,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6912D463-5787-4386-AC5E-483DCEEE662E}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,6 +913,23 @@
       </c>
       <c r="E7" s="2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1097,29 +1127,29 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="12">
         <v>16</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="15" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10" t="s">
+      <c r="A18" s="13"/>
+      <c r="B18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13" t="s">
+      <c r="A19" s="14"/>
+      <c r="B19" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="14"/>
+      <c r="C19" s="17"/>
     </row>
     <row r="20" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
@@ -1133,41 +1163,41 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="A21" s="12">
         <v>18</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="15" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="16" t="s">
+      <c r="A22" s="13"/>
+      <c r="B22" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="11"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="16" t="s">
+      <c r="A23" s="13"/>
+      <c r="B23" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="11"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
-      <c r="B25" s="17" t="s">
+      <c r="A25" s="14"/>
+      <c r="B25" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="14"/>
+      <c r="C25" s="17"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">

</xml_diff>